<commit_message>
Sun Dec  8 09:51:33 PM EST 2024
</commit_message>
<xml_diff>
--- a/xgboost_params.xlsx
+++ b/xgboost_params.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,21 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>iron VDZP</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ltneg5 joint VDZP</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ltneg4 joint VDZP</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>joint VDZP</t>
         </is>
       </c>
@@ -491,6 +506,21 @@
           <t>reg:squarederror</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>reg:squarederror</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>reg:squarederror</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>reg:squarederror</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -513,6 +543,15 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -535,6 +574,15 @@
       <c r="F4" t="n">
         <v>10</v>
       </c>
+      <c r="G4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H4" t="n">
+        <v>100</v>
+      </c>
+      <c r="I4" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -555,7 +603,16 @@
         <v>100</v>
       </c>
       <c r="F5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G5" t="n">
         <v>100</v>
+      </c>
+      <c r="H5" t="n">
+        <v>100</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="6">
@@ -579,6 +636,15 @@
       <c r="F6" t="n">
         <v>0.001</v>
       </c>
+      <c r="G6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -600,6 +666,15 @@
       </c>
       <c r="F7" t="n">
         <v>0.001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tue Feb  4 06:29:16 PM EST 2025
</commit_message>
<xml_diff>
--- a/xgboost_params.xlsx
+++ b/xgboost_params.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,42 +436,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>H2n VDZP</t>
+          <t>H2n</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>iron VDZP</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ozone MB</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>ozone VDZP</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>ozone VTZP</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>ozone MB</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>iron VDZP</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ltneg5 joint VDZP</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>ltneg4 joint VDZP</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>joint VDZP</t>
         </is>
       </c>
     </row>
@@ -506,21 +491,6 @@
           <t>reg:squarederror</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>reg:squarederror</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>reg:squarederror</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>reg:squarederror</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -543,15 +513,6 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -563,24 +524,15 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D4" t="n">
         <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
-      </c>
-      <c r="G4" t="n">
-        <v>10</v>
-      </c>
-      <c r="H4" t="n">
-        <v>100</v>
-      </c>
-      <c r="I4" t="n">
         <v>10</v>
       </c>
     </row>
@@ -591,7 +543,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C5" t="n">
         <v>100</v>
@@ -603,16 +555,7 @@
         <v>100</v>
       </c>
       <c r="F5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G5" t="n">
         <v>100</v>
-      </c>
-      <c r="H5" t="n">
-        <v>100</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1000</v>
       </c>
     </row>
     <row r="6">
@@ -622,28 +565,19 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>1e-06</v>
+      </c>
+      <c r="C6" t="n">
         <v>0.001</v>
       </c>
-      <c r="C6" t="n">
-        <v>1e-06</v>
-      </c>
       <c r="D6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.001</v>
       </c>
       <c r="F6" t="n">
         <v>0.001</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.1</v>
       </c>
     </row>
     <row r="7">
@@ -653,10 +587,10 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C7" t="n">
         <v>0.1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1e-06</v>
       </c>
       <c r="D7" t="n">
         <v>0.1</v>
@@ -666,15 +600,6 @@
       </c>
       <c r="F7" t="n">
         <v>0.001</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>